<commit_message>
added events functionality stable
</commit_message>
<xml_diff>
--- a/Chat_Feature_Log.xlsx
+++ b/Chat_Feature_Log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>Main Screen</t>
   </si>
@@ -128,9 +128,6 @@
     <t>View Resource - Upload</t>
   </si>
   <si>
-    <t>View Resource - Link</t>
-  </si>
-  <si>
     <t>Create Resource - Contact</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Comment when voting in a poll</t>
   </si>
   <si>
-    <t>Group Chat - Display message when poll/resource is added</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -171,6 +165,21 @@
   </si>
   <si>
     <t>Events</t>
+  </si>
+  <si>
+    <t>Joined Group List screen separate to current group screen</t>
+  </si>
+  <si>
+    <t>Registration ask for Country</t>
+  </si>
+  <si>
+    <t>Groups to be country specific</t>
+  </si>
+  <si>
+    <t>Group Chat - Improve System updates vs users chat (keep them separate)</t>
+  </si>
+  <si>
+    <t>View Resource - Link - is this really required?</t>
   </si>
 </sst>
 </file>
@@ -202,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,11 +243,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +530,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
@@ -779,7 +795,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -787,7 +803,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
@@ -798,7 +814,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -809,7 +825,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -820,7 +836,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
@@ -828,10 +844,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
         <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -839,10 +855,10 @@
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
@@ -851,10 +867,10 @@
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -862,59 +878,92 @@
     </row>
     <row r="30" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="3" t="s">
+    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
+    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ionic version 5 + link upload working
</commit_message>
<xml_diff>
--- a/Chat_Feature_Log.xlsx
+++ b/Chat_Feature_Log.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$37</definedName>
   </definedNames>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
@@ -140,9 +140,6 @@
     <t>Features</t>
   </si>
   <si>
-    <t>Group Chat - Tag a message a resource</t>
-  </si>
-  <si>
     <t>Rate Resources and Write a comment</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>View Resource - Link - is this really required?</t>
+  </si>
+  <si>
+    <t>Group Message menu - tag resource, report inappropriate etc</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,7 +795,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -803,7 +803,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
@@ -842,14 +842,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -858,7 +858,7 @@
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
@@ -870,7 +870,7 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -881,7 +881,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>7</v>
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>8</v>
@@ -903,21 +903,21 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -925,10 +925,10 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -939,7 +939,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -950,7 +950,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -961,14 +961,14 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F34">
+  <autoFilter ref="A1:F37">
     <filterColumn colId="3">
       <filters>
         <filter val="InProgress"/>

</xml_diff>

<commit_message>
posts implemented (without ion-card)
</commit_message>
<xml_diff>
--- a/Chat_Feature_Log.xlsx
+++ b/Chat_Feature_Log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
   <si>
     <t>Main Screen</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Pin a resource</t>
   </si>
   <si>
-    <t>Broadcast?</t>
-  </si>
-  <si>
     <t>Comment when voting in a poll</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>Events</t>
   </si>
   <si>
-    <t>Joined Group List screen separate to current group screen</t>
-  </si>
-  <si>
     <t>Registration ask for Country</t>
   </si>
   <si>
@@ -176,10 +170,22 @@
     <t>Group Chat - Improve System updates vs users chat (keep them separate)</t>
   </si>
   <si>
-    <t>View Resource - Link - is this really required?</t>
-  </si>
-  <si>
     <t>Group Message menu - tag resource, report inappropriate etc</t>
+  </si>
+  <si>
+    <t>View Resource - Link</t>
+  </si>
+  <si>
+    <t>Create webcomponent for nested comments</t>
+  </si>
+  <si>
+    <t>User Group member List screen should be separate to current group screen</t>
+  </si>
+  <si>
+    <t>Create posts (rather than group messages)</t>
+  </si>
+  <si>
+    <t>Broadcast or call it Announcements!</t>
   </si>
 </sst>
 </file>
@@ -530,16 +536,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -776,7 +782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -784,7 +790,7 @@
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -795,18 +801,18 @@
         <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
@@ -831,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -839,17 +845,17 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -870,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -892,7 +898,7 @@
         <v>36</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>8</v>
@@ -903,7 +909,7 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
@@ -914,7 +920,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>7</v>
@@ -925,10 +931,10 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -939,7 +945,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -950,7 +956,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -961,10 +967,32 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>